<commit_message>
-Table format changes  *Font, Color, Border, Spacing
</commit_message>
<xml_diff>
--- a/report_2021.xlsx
+++ b/report_2021.xlsx
@@ -16,9 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+  <numFmts count="1">
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="164"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -32,15 +31,21 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C0C0C0"/>
+        <bgColor rgb="00C0C0C0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -54,18 +59,39 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf applyAlignment="1" borderId="2" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="2" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -140,6 +166,825 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Impulse Noise Evaluation</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <lineChart>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Report'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$B$2:$B$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Report'!C1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$C$2:$C$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <strRef>
+              <f>'Report'!D1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$D$2:$D$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <strRef>
+              <f>'Report'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$E$2:$E$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <strRef>
+              <f>'Report'!F1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$F$2:$F$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <strRef>
+              <f>'Report'!G1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$G$2:$G$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <strRef>
+              <f>'Report'!H1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$H$2:$H$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <strRef>
+              <f>'Report'!I1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$I$2:$I$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <strRef>
+              <f>'Report'!J1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$J$2:$J$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="9"/>
+          <order val="9"/>
+          <tx>
+            <strRef>
+              <f>'Report'!K1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$K$2:$K$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="10"/>
+          <order val="10"/>
+          <tx>
+            <strRef>
+              <f>'Report'!L1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$L$2:$L$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="11"/>
+          <order val="11"/>
+          <tx>
+            <strRef>
+              <f>'Report'!M1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$M$2:$M$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="12"/>
+          <order val="12"/>
+          <tx>
+            <strRef>
+              <f>'Report'!N1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$N$2:$N$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="13"/>
+          <order val="13"/>
+          <tx>
+            <strRef>
+              <f>'Report'!O1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$O$2:$O$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="14"/>
+          <order val="14"/>
+          <tx>
+            <strRef>
+              <f>'Report'!P1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$P$2:$P$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="15"/>
+          <order val="15"/>
+          <tx>
+            <strRef>
+              <f>'Report'!Q1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$Q$2:$Q$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="16"/>
+          <order val="16"/>
+          <tx>
+            <strRef>
+              <f>'Report'!R1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$R$2:$R$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="17"/>
+          <order val="17"/>
+          <tx>
+            <strRef>
+              <f>'Report'!S1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$S$2:$S$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="18"/>
+          <order val="18"/>
+          <tx>
+            <strRef>
+              <f>'Report'!T1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$T$2:$T$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="19"/>
+          <order val="19"/>
+          <tx>
+            <strRef>
+              <f>'Report'!U1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$U$2:$U$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="20"/>
+          <order val="20"/>
+          <tx>
+            <strRef>
+              <f>'Report'!V1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$V$2:$V$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="21"/>
+          <order val="21"/>
+          <tx>
+            <strRef>
+              <f>'Report'!W1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <cat>
+            <numRef>
+              <f>'Report'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$W$2:$W$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <axId val="10"/>
+        <axId val="100"/>
+      </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Test Shot</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500">
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr sz="1500">
+              <a:latin typeface="Calibri"/>
+            </a:endParaRPr>
+          </a:p>
+        </txPr>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9000000" cy="4680000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -426,350 +1271,376 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A5:W8"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="21.6"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
+    <col customWidth="1" max="3" min="3" width="22.8"/>
+    <col customWidth="1" max="4" min="4" width="16.8"/>
+    <col customWidth="1" max="5" min="5" width="27.6"/>
+    <col customWidth="1" max="6" min="6" width="16.8"/>
+    <col customWidth="1" max="7" min="7" width="27.6"/>
+    <col customWidth="1" max="8" min="8" width="26.4"/>
+    <col customWidth="1" max="9" min="9" width="22.8"/>
+    <col customWidth="1" max="10" min="10" width="33.6"/>
+    <col customWidth="1" max="11" min="11" width="24"/>
+    <col customWidth="1" max="12" min="12" width="34.8"/>
+    <col customWidth="1" max="13" min="13" width="19.2"/>
+    <col customWidth="1" max="14" min="14" width="15.6"/>
+    <col customWidth="1" max="15" min="15" width="15.6"/>
+    <col customWidth="1" max="16" min="16" width="25.2"/>
+    <col customWidth="1" max="17" min="17" width="25.2"/>
+    <col customWidth="1" max="18" min="18" width="19.2"/>
+    <col customWidth="1" max="19" min="19" width="31.2"/>
+    <col customWidth="1" max="20" min="20" width="31.2"/>
+    <col customWidth="1" max="21" min="21" width="31.2"/>
+    <col customWidth="1" max="22" min="22" width="73.2"/>
+    <col customWidth="1" max="23" min="23" width="73.2"/>
+  </cols>
   <sheetData>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Measurement time</t>
         </is>
       </c>
-      <c r="B5" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>01. Peak</t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>01. Peak position</t>
         </is>
       </c>
-      <c r="D5" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>02. 90% peak</t>
         </is>
       </c>
-      <c r="E5" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>02. 90% peak position</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>03. 10% peak</t>
         </is>
       </c>
-      <c r="G5" s="1" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>03. 10% peak position</t>
         </is>
       </c>
-      <c r="H5" s="1" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>04. Signal rise time</t>
         </is>
       </c>
-      <c r="I5" s="1" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>05. 10% peak left</t>
         </is>
       </c>
-      <c r="J5" s="1" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>05. 10% peak left position</t>
         </is>
       </c>
-      <c r="K5" s="1" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>06. 10% peak right</t>
         </is>
       </c>
-      <c r="L5" s="1" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>06. 10% peak right position</t>
         </is>
       </c>
-      <c r="M5" s="1" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>07. A-duration</t>
         </is>
       </c>
-      <c r="N5" s="1" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>08. L+ line</t>
         </is>
       </c>
-      <c r="O5" s="1" t="inlineStr">
+      <c r="O1" s="3" t="inlineStr">
         <is>
           <t>09. L- line</t>
         </is>
       </c>
-      <c r="P5" s="1" t="inlineStr">
+      <c r="P1" s="3" t="inlineStr">
         <is>
           <t>10. P time position</t>
         </is>
       </c>
-      <c r="Q5" s="1" t="inlineStr">
+      <c r="Q1" s="3" t="inlineStr">
         <is>
           <t>11. Primary portion</t>
         </is>
       </c>
-      <c r="R5" s="1" t="inlineStr">
+      <c r="R1" s="3" t="inlineStr">
         <is>
           <t>12. B-duration</t>
         </is>
       </c>
-      <c r="S5" s="1" t="inlineStr">
+      <c r="S1" s="3" t="inlineStr">
         <is>
           <t>13. Fluctuation duration</t>
         </is>
       </c>
-      <c r="T5" s="1" t="inlineStr">
+      <c r="T1" s="3" t="inlineStr">
         <is>
           <t>15. Sound Exposure Level</t>
         </is>
       </c>
-      <c r="U5" s="1" t="inlineStr">
+      <c r="U1" s="3" t="inlineStr">
         <is>
           <t>16. Sound Pressure Level</t>
         </is>
       </c>
-      <c r="V5" s="1" t="inlineStr">
+      <c r="V1" s="3" t="inlineStr">
         <is>
           <t>17. N1 - allowable number of impulses/day (single protect.)</t>
         </is>
       </c>
-      <c r="W5" s="1" t="inlineStr">
+      <c r="W1" s="3" t="inlineStr">
         <is>
           <t>18. N2 - allowable number of impulses/day (double protect.)</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
+    <row r="2">
+      <c r="A2" s="4" t="n">
         <v>44426.53980324074</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B2" s="5" t="n">
         <v>70.60208608974546</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C2" s="5" t="n">
         <v>0.06341743526385001</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D2" s="5" t="n">
         <v>69.6869362785322</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E2" s="5" t="n">
         <v>0.06341476121616114</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F2" s="5" t="n">
         <v>50.60208608974562</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G2" s="5" t="n">
         <v>0.06333210447282564</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H2" s="5" t="n">
         <v>0.08265674333551135</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I2" s="5" t="n">
         <v>50.60208608974562</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J2" s="5" t="n">
         <v>0.06333210447282564</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K2" s="5" t="n">
         <v>50.60208608974562</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L2" s="5" t="n">
         <v>0.06344357885081084</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M2" s="5" t="n">
         <v>0.111474379991705</v>
       </c>
-      <c r="N6" t="n">
+      <c r="N2" s="5" t="n">
         <v>50.60208627598737</v>
       </c>
-      <c r="O6" t="n">
+      <c r="O2" s="5" t="n">
         <v>54.49703911733203</v>
       </c>
-      <c r="P6" t="n">
+      <c r="P2" s="5" t="n">
         <v>0.0639627207972152</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="Q2" s="5" t="n">
         <v>0.630616324333212</v>
       </c>
-      <c r="R6" t="n">
+      <c r="R2" s="5" t="n">
         <v>25.7122510718332</v>
       </c>
-      <c r="S6" t="n">
+      <c r="S2" s="5" t="n">
         <v>25.0816347475</v>
       </c>
-      <c r="T6" t="n">
+      <c r="T2" s="5" t="n">
         <v>40.18205560149801</v>
       </c>
-      <c r="U6" t="n">
+      <c r="U2" s="5" t="n">
         <v>57.6770948181196</v>
       </c>
-      <c r="V6" t="n">
+      <c r="V2" s="5" t="n">
         <v>1.24582641804343e+30</v>
       </c>
-      <c r="W6" t="n">
+      <c r="W2" s="5" t="n">
         <v>2.491652836086856e+31</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
+    <row r="3">
+      <c r="A3" s="4" t="n">
         <v>44426.57805555555</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B3" s="5" t="n">
         <v>69.81411036687045</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C3" s="5" t="n">
         <v>0.05328178453775</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D3" s="5" t="n">
         <v>68.8989605556572</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E3" s="5" t="n">
         <v>0.0532800600607366</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F3" s="5" t="n">
         <v>49.81411036687051</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G3" s="5" t="n">
         <v>0.05326320803506999</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H3" s="5" t="n">
         <v>0.01685202566658813</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I3" s="5" t="n">
         <v>49.81411036687051</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J3" s="5" t="n">
         <v>0.05326320803506999</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K3" s="5" t="n">
         <v>49.81411036687051</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L3" s="5" t="n">
         <v>0.0532932304555799</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M3" s="5" t="n">
         <v>0.03002242101501905</v>
       </c>
-      <c r="N7" t="n">
+      <c r="N3" s="5" t="n">
         <v>49.81411047707999</v>
       </c>
-      <c r="O7" t="n">
+      <c r="O3" s="5" t="n">
         <v>51.2566328683866</v>
       </c>
-      <c r="P7" t="n">
+      <c r="P3" s="5" t="n">
         <v>0.0534281250810034</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="Q3" s="5" t="n">
         <v>0.1649170459282898</v>
       </c>
-      <c r="R7" t="n">
+      <c r="R3" s="5" t="n">
         <v>33.32417332617828</v>
       </c>
-      <c r="S7" t="n">
+      <c r="S3" s="5" t="n">
         <v>33.15925628025</v>
       </c>
-      <c r="T7" t="n">
+      <c r="T3" s="5" t="n">
         <v>40.07565120932365</v>
       </c>
-      <c r="U7" t="n">
+      <c r="U3" s="5" t="n">
         <v>58.46015756704364</v>
       </c>
-      <c r="V7" t="n">
+      <c r="V3" s="5" t="n">
         <v>1.229157951070582e+30</v>
       </c>
-      <c r="W7" t="n">
+      <c r="W3" s="5" t="n">
         <v>2.458315902141163e+31</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
+    <row r="4">
+      <c r="A4" s="4" t="n">
         <v>44426.62946759259</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B4" s="5" t="n">
         <v>74.38578822806605</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C4" s="5" t="n">
         <v>0.0546531682171</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D4" s="5" t="n">
         <v>73.4706384168523</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E4" s="5" t="n">
         <v>0.05465176980655854</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F4" s="5" t="n">
         <v>54.38578822806593</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G4" s="5" t="n">
         <v>0.05464445219883175</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H4" s="5" t="n">
         <v>0.007317607726792245</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I4" s="5" t="n">
         <v>54.38578822806593</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J4" s="5" t="n">
         <v>0.05464445219883175</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K4" s="5" t="n">
         <v>54.38578822806593</v>
       </c>
-      <c r="L8" t="n">
+      <c r="L4" s="5" t="n">
         <v>0.05466492865880135</v>
       </c>
-      <c r="M8" t="n">
+      <c r="M4" s="5" t="n">
         <v>0.0204764601221541</v>
       </c>
-      <c r="N8" t="n">
+      <c r="N4" s="5" t="n">
         <v>54.38578817539481</v>
       </c>
-      <c r="O8" t="n">
+      <c r="O4" s="5" t="n">
         <v>55.58368821303939</v>
       </c>
-      <c r="P8" t="n">
+      <c r="P4" s="5" t="n">
         <v>0.05480354926886775</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="Q4" s="5" t="n">
         <v>0.1590970700410048</v>
       </c>
-      <c r="R8" t="n">
+      <c r="R4" s="5" t="n">
         <v>29.88703312894101</v>
       </c>
-      <c r="S8" t="n">
+      <c r="S4" s="5" t="n">
         <v>29.7279360589</v>
       </c>
-      <c r="T8" t="n">
+      <c r="T4" s="5" t="n">
         <v>42.63544114063679</v>
       </c>
-      <c r="U8" t="n">
+      <c r="U4" s="5" t="n">
         <v>61.59048725826955</v>
       </c>
-      <c r="V8" t="n">
+      <c r="V4" s="5" t="n">
         <v>8.22843537808425e+29</v>
       </c>
-      <c r="W8" t="n">
+      <c r="W4" s="5" t="n">
         <v>1.64568707561685e+31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>